<commit_message>
endret noe tekst, forsøk på tabell, standard avvik x2, lagt inn graf
</commit_message>
<xml_diff>
--- a/data/g2.xlsx
+++ b/data/g2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Idrettsvitenskap/MASTER/Prosjekt Vo2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01-projects\Gruppeoppgave-1-gruppe1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2459FA4-E049-2845-A42F-CA1D644D7ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14FEB5F-5117-4EE8-9CC1-F9525585FC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{7E94264A-058A-1B4C-853F-B20CD5202A47}"/>
+    <workbookView xWindow="2424" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{7E94264A-058A-1B4C-853F-B20CD5202A47}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="plotting"/>
@@ -300,9 +300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,7 +340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -446,7 +446,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -588,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,12 +599,12 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -728,7 +728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -790,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>[1]plotting!D4</f>
         <v>5</v>
@@ -871,7 +871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -933,7 +933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -995,7 +995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1101,10 +1101,10 @@
         <v>5747</v>
       </c>
       <c r="O8">
+        <v>1.125</v>
+      </c>
+      <c r="P8">
         <v>160.5</v>
-      </c>
-      <c r="P8">
-        <v>1.125</v>
       </c>
       <c r="Q8">
         <v>39.700000000000003</v>
@@ -1119,7 +1119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1367,57 +1367,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
la til 2 grafer, endret tekst, la til i YAML- code-fod, warning false og message false. limte inn protokoll og endret på kjønn i exel slik at alle sier det samme
</commit_message>
<xml_diff>
--- a/data/g2.xlsx
+++ b/data/g2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01-projects\Gruppeoppgave-1-gruppe1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\#prosjekt_R\Gruppeoppgave-1-gruppe1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14FEB5F-5117-4EE8-9CC1-F9525585FC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734BB4A1-1088-4F0D-BB65-261F2D75898D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{7E94264A-058A-1B4C-853F-B20CD5202A47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E94264A-058A-1B4C-853F-B20CD5202A47}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -107,9 +107,6 @@
     <t>t3</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -119,13 +116,13 @@
     <t>t2</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
-    <t>F</t>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -204,11 +201,6 @@
         <row r="4">
           <cell r="D4">
             <v>5</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>M</v>
           </cell>
         </row>
         <row r="6">
@@ -599,12 +591,12 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -689,7 +681,7 @@
         <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I2">
         <v>27.956164383561642</v>
@@ -719,7 +711,7 @@
         <v>64.2</v>
       </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S2" s="4">
         <v>14.51</v>
@@ -728,7 +720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -736,7 +728,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <v>45546</v>
@@ -751,7 +743,7 @@
         <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I3">
         <v>27.961643835616439</v>
@@ -790,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>[1]plotting!D4</f>
         <v>5</v>
@@ -818,9 +810,8 @@
         <f>[1]plotting!D19</f>
         <v>66</v>
       </c>
-      <c r="H4" t="str">
-        <f>[1]plotting!D5</f>
-        <v>M</v>
+      <c r="H4" t="s">
+        <v>26</v>
       </c>
       <c r="I4">
         <f>IF(AND([1]plotting!$D$6&gt;0,[1]plotting!$D$12&gt;0),([1]plotting!$D$12-[1]plotting!$D$6)/365,"na")</f>
@@ -871,7 +862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -879,7 +870,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1">
         <v>45533</v>
@@ -894,7 +885,7 @@
         <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5">
         <v>23.186301369863013</v>
@@ -933,7 +924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -941,7 +932,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1">
         <v>45533</v>
@@ -956,7 +947,7 @@
         <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6">
         <v>23.389041095890413</v>
@@ -995,7 +986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1003,7 +994,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1">
         <v>45531</v>
@@ -1018,7 +1009,7 @@
         <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7">
         <v>23.383561643835616</v>
@@ -1057,7 +1048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1065,7 +1056,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>45531</v>
@@ -1080,7 +1071,7 @@
         <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I8">
         <v>24.213698630136985</v>
@@ -1119,7 +1110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1127,7 +1118,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>45533</v>
@@ -1142,7 +1133,7 @@
         <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I9">
         <v>24.219178082191782</v>
@@ -1175,13 +1166,13 @@
         <v>191</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T9">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1204,7 +1195,7 @@
         <v>82</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I10">
         <v>24.24931506849315</v>
@@ -1243,7 +1234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1251,7 +1242,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1">
         <v>45546</v>
@@ -1266,7 +1257,7 @@
         <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I11">
         <v>24.254794520547946</v>
@@ -1305,7 +1296,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1313,7 +1304,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1">
         <v>45546</v>
@@ -1328,7 +1319,7 @@
         <v>52</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12">
         <v>43.717808219178082</v>
@@ -1367,57 +1358,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
     </row>
   </sheetData>

</xml_diff>